<commit_message>
Delete "Soustředění na hru"
</commit_message>
<xml_diff>
--- a/docs/csv/diagnostika_sheet1.xlsx
+++ b/docs/csv/diagnostika_sheet1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1974" uniqueCount="553">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1962" uniqueCount="552">
   <si>
     <t xml:space="preserve">temporary_task_id</t>
   </si>
@@ -1508,9 +1508,6 @@
   </si>
   <si>
     <t xml:space="preserve">Při hrách uplatňuje iniciativu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Soustředení na hru</t>
   </si>
   <si>
     <t xml:space="preserve">Musí být upozorněno</t>
@@ -1818,10 +1815,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K451"/>
+  <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A370" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B402" activeCellId="0" sqref="B402"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.12890625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11654,28 +11651,25 @@
     </row>
     <row r="398" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A398" s="1" t="n">
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="C398" s="1" t="n">
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="D398" s="1" t="s">
         <v>496</v>
       </c>
       <c r="E398" s="1" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="F398" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F398" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="H398" s="1" t="n">
-        <v>1</v>
-      </c>
       <c r="I398" s="1" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="J398" s="1" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="K398" s="2" t="s">
         <v>14</v>
@@ -11683,28 +11677,22 @@
     </row>
     <row r="399" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A399" s="1" t="n">
-        <v>398</v>
-      </c>
-      <c r="B399" s="1" t="n">
-        <v>397</v>
+        <v>401</v>
+      </c>
+      <c r="C399" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="D399" s="1" t="s">
-        <v>496</v>
+        <v>499</v>
       </c>
       <c r="E399" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="F399" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="H399" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I399" s="1" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="J399" s="1" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="K399" s="2" t="s">
         <v>14</v>
@@ -11712,28 +11700,22 @@
     </row>
     <row r="400" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A400" s="1" t="n">
-        <v>399</v>
-      </c>
-      <c r="B400" s="1" t="n">
-        <v>397</v>
+        <v>402</v>
+      </c>
+      <c r="C400" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="D400" s="1" t="s">
-        <v>496</v>
+        <v>500</v>
       </c>
       <c r="E400" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="F400" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="H400" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I400" s="1" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="J400" s="1" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="K400" s="2" t="s">
         <v>14</v>
@@ -11741,25 +11723,25 @@
     </row>
     <row r="401" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A401" s="1" t="n">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="C401" s="1" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D401" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="E401" s="1" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="F401" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="I401" s="1" t="s">
         <v>497</v>
       </c>
-      <c r="E401" s="1" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="F401" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="I401" s="1" t="s">
+      <c r="J401" s="1" t="s">
         <v>498</v>
-      </c>
-      <c r="J401" s="1" t="s">
-        <v>499</v>
       </c>
       <c r="K401" s="2" t="s">
         <v>14</v>
@@ -11767,22 +11749,25 @@
     </row>
     <row r="402" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A402" s="1" t="n">
-        <v>401</v>
+        <v>404</v>
       </c>
       <c r="C402" s="1" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D402" s="1" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="E402" s="1" t="n">
-        <v>3</v>
+        <v>3.5</v>
+      </c>
+      <c r="F402" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="I402" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="J402" s="1" t="s">
         <v>498</v>
-      </c>
-      <c r="J402" s="1" t="s">
-        <v>499</v>
       </c>
       <c r="K402" s="2" t="s">
         <v>14</v>
@@ -11790,22 +11775,25 @@
     </row>
     <row r="403" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A403" s="1" t="n">
-        <v>402</v>
+        <v>405</v>
       </c>
       <c r="C403" s="1" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D403" s="1" t="s">
-        <v>501</v>
+        <v>504</v>
       </c>
       <c r="E403" s="1" t="n">
         <v>4</v>
       </c>
+      <c r="F403" s="1" t="n">
+        <v>5</v>
+      </c>
       <c r="I403" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="J403" s="1" t="s">
         <v>498</v>
-      </c>
-      <c r="J403" s="1" t="s">
-        <v>499</v>
       </c>
       <c r="K403" s="2" t="s">
         <v>14</v>
@@ -11813,25 +11801,25 @@
     </row>
     <row r="404" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A404" s="1" t="n">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="C404" s="1" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D404" s="1" t="s">
-        <v>502</v>
+        <v>505</v>
       </c>
       <c r="E404" s="1" t="n">
-        <v>3.5</v>
+        <v>5</v>
       </c>
       <c r="F404" s="1" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I404" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="J404" s="1" t="s">
         <v>498</v>
-      </c>
-      <c r="J404" s="1" t="s">
-        <v>499</v>
       </c>
       <c r="K404" s="2" t="s">
         <v>14</v>
@@ -11839,13 +11827,13 @@
     </row>
     <row r="405" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A405" s="1" t="n">
-        <v>404</v>
+        <v>407</v>
       </c>
       <c r="C405" s="1" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D405" s="1" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
       <c r="E405" s="1" t="n">
         <v>3.5</v>
@@ -11854,10 +11842,10 @@
         <v>4</v>
       </c>
       <c r="I405" s="1" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="J405" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="K405" s="2" t="s">
         <v>14</v>
@@ -11865,25 +11853,25 @@
     </row>
     <row r="406" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A406" s="1" t="n">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="C406" s="1" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D406" s="1" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="E406" s="1" t="n">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="F406" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I406" s="1" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="J406" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="K406" s="2" t="s">
         <v>14</v>
@@ -11891,25 +11879,25 @@
     </row>
     <row r="407" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A407" s="1" t="n">
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="C407" s="1" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D407" s="1" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="E407" s="1" t="n">
-        <v>5</v>
+        <v>3.5</v>
       </c>
       <c r="F407" s="1" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I407" s="1" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="J407" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="K407" s="2" t="s">
         <v>14</v>
@@ -11917,25 +11905,22 @@
     </row>
     <row r="408" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A408" s="1" t="n">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="C408" s="1" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D408" s="1" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="E408" s="1" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="F408" s="1" t="n">
         <v>4</v>
       </c>
       <c r="I408" s="1" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="J408" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="K408" s="2" t="s">
         <v>14</v>
@@ -11943,25 +11928,25 @@
     </row>
     <row r="409" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A409" s="1" t="n">
-        <v>408</v>
+        <v>411</v>
       </c>
       <c r="C409" s="1" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D409" s="1" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="E409" s="1" t="n">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="F409" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I409" s="1" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="J409" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="K409" s="2" t="s">
         <v>14</v>
@@ -11969,25 +11954,22 @@
     </row>
     <row r="410" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A410" s="1" t="n">
-        <v>409</v>
+        <v>412</v>
       </c>
       <c r="C410" s="1" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D410" s="1" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="E410" s="1" t="n">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="F410" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I410" s="1" t="s">
-        <v>504</v>
-      </c>
-      <c r="J410" s="1" t="s">
-        <v>499</v>
+        <v>503</v>
       </c>
       <c r="K410" s="2" t="s">
         <v>14</v>
@@ -11995,22 +11977,25 @@
     </row>
     <row r="411" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A411" s="1" t="n">
-        <v>410</v>
+        <v>413</v>
       </c>
       <c r="C411" s="1" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D411" s="1" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="E411" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="F411" s="1" t="n">
+        <v>6</v>
       </c>
       <c r="I411" s="1" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="J411" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="K411" s="2" t="s">
         <v>14</v>
@@ -12018,25 +12003,22 @@
     </row>
     <row r="412" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A412" s="1" t="n">
-        <v>411</v>
+        <v>414</v>
       </c>
       <c r="C412" s="1" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D412" s="1" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="E412" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="F412" s="1" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I412" s="1" t="s">
-        <v>504</v>
+        <v>514</v>
       </c>
       <c r="J412" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="K412" s="2" t="s">
         <v>14</v>
@@ -12044,22 +12026,22 @@
     </row>
     <row r="413" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A413" s="1" t="n">
-        <v>412</v>
+        <v>415</v>
       </c>
       <c r="C413" s="1" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D413" s="1" t="s">
-        <v>512</v>
+        <v>515</v>
       </c>
       <c r="E413" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="F413" s="1" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I413" s="1" t="s">
-        <v>504</v>
+        <v>514</v>
+      </c>
+      <c r="J413" s="1" t="s">
+        <v>498</v>
       </c>
       <c r="K413" s="2" t="s">
         <v>14</v>
@@ -12067,25 +12049,22 @@
     </row>
     <row r="414" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A414" s="1" t="n">
-        <v>413</v>
+        <v>416</v>
       </c>
       <c r="C414" s="1" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D414" s="1" t="s">
-        <v>513</v>
+        <v>516</v>
       </c>
       <c r="E414" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="F414" s="1" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I414" s="1" t="s">
-        <v>504</v>
+        <v>514</v>
       </c>
       <c r="J414" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="K414" s="2" t="s">
         <v>14</v>
@@ -12093,22 +12072,22 @@
     </row>
     <row r="415" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A415" s="1" t="n">
-        <v>414</v>
+        <v>417</v>
       </c>
       <c r="C415" s="1" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D415" s="1" t="s">
-        <v>514</v>
+        <v>517</v>
       </c>
       <c r="E415" s="1" t="n">
         <v>3</v>
       </c>
       <c r="I415" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="J415" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="K415" s="2" t="s">
         <v>14</v>
@@ -12116,22 +12095,25 @@
     </row>
     <row r="416" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A416" s="1" t="n">
-        <v>415</v>
+        <v>418</v>
       </c>
       <c r="C416" s="1" t="n">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D416" s="1" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="E416" s="1" t="n">
         <v>3</v>
       </c>
+      <c r="F416" s="1" t="n">
+        <v>4</v>
+      </c>
       <c r="I416" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="J416" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="K416" s="2" t="s">
         <v>14</v>
@@ -12139,22 +12121,25 @@
     </row>
     <row r="417" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A417" s="1" t="n">
-        <v>416</v>
+        <v>419</v>
       </c>
       <c r="C417" s="1" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D417" s="1" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="E417" s="1" t="n">
         <v>3</v>
       </c>
+      <c r="F417" s="1" t="n">
+        <v>4</v>
+      </c>
       <c r="I417" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="J417" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="K417" s="2" t="s">
         <v>14</v>
@@ -12162,22 +12147,25 @@
     </row>
     <row r="418" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A418" s="1" t="n">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="C418" s="1" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D418" s="1" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="E418" s="1" t="n">
         <v>3</v>
       </c>
+      <c r="F418" s="1" t="n">
+        <v>4</v>
+      </c>
       <c r="I418" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="J418" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="K418" s="2" t="s">
         <v>14</v>
@@ -12185,25 +12173,22 @@
     </row>
     <row r="419" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A419" s="1" t="n">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c r="C419" s="1" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D419" s="1" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="E419" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="F419" s="1" t="n">
         <v>4</v>
       </c>
       <c r="I419" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="J419" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="K419" s="2" t="s">
         <v>14</v>
@@ -12211,25 +12196,22 @@
     </row>
     <row r="420" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A420" s="1" t="n">
-        <v>419</v>
+        <v>422</v>
       </c>
       <c r="C420" s="1" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D420" s="1" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="E420" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="F420" s="1" t="n">
         <v>4</v>
       </c>
       <c r="I420" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="J420" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="K420" s="2" t="s">
         <v>14</v>
@@ -12237,25 +12219,22 @@
     </row>
     <row r="421" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A421" s="1" t="n">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c r="C421" s="1" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D421" s="1" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="E421" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="F421" s="1" t="n">
         <v>4</v>
       </c>
       <c r="I421" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="J421" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="K421" s="2" t="s">
         <v>14</v>
@@ -12263,22 +12242,22 @@
     </row>
     <row r="422" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A422" s="1" t="n">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="C422" s="1" t="n">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D422" s="1" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="E422" s="1" t="n">
         <v>4</v>
       </c>
       <c r="I422" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="J422" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="K422" s="2" t="s">
         <v>14</v>
@@ -12286,22 +12265,22 @@
     </row>
     <row r="423" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A423" s="1" t="n">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="C423" s="1" t="n">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D423" s="1" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="E423" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I423" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="J423" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="K423" s="2" t="s">
         <v>14</v>
@@ -12309,22 +12288,22 @@
     </row>
     <row r="424" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A424" s="1" t="n">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="C424" s="1" t="n">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D424" s="1" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c r="E424" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I424" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="J424" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="K424" s="2" t="s">
         <v>14</v>
@@ -12332,22 +12311,22 @@
     </row>
     <row r="425" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A425" s="1" t="n">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="C425" s="1" t="n">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D425" s="1" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="E425" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I425" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="J425" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="K425" s="2" t="s">
         <v>14</v>
@@ -12355,22 +12334,22 @@
     </row>
     <row r="426" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A426" s="1" t="n">
-        <v>425</v>
+        <v>428</v>
       </c>
       <c r="C426" s="1" t="n">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D426" s="1" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="E426" s="1" t="n">
         <v>5</v>
       </c>
       <c r="I426" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="J426" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="K426" s="2" t="s">
         <v>14</v>
@@ -12378,22 +12357,22 @@
     </row>
     <row r="427" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A427" s="1" t="n">
-        <v>426</v>
+        <v>429</v>
       </c>
       <c r="C427" s="1" t="n">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D427" s="1" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="E427" s="1" t="n">
         <v>5</v>
       </c>
       <c r="I427" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="J427" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="K427" s="2" t="s">
         <v>14</v>
@@ -12401,22 +12380,22 @@
     </row>
     <row r="428" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A428" s="1" t="n">
-        <v>427</v>
+        <v>430</v>
       </c>
       <c r="C428" s="1" t="n">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D428" s="1" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="E428" s="1" t="n">
         <v>5</v>
       </c>
       <c r="I428" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="J428" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="K428" s="2" t="s">
         <v>14</v>
@@ -12424,22 +12403,22 @@
     </row>
     <row r="429" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A429" s="1" t="n">
-        <v>428</v>
+        <v>431</v>
       </c>
       <c r="C429" s="1" t="n">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D429" s="1" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="E429" s="1" t="n">
         <v>5</v>
       </c>
       <c r="I429" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="J429" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="K429" s="2" t="s">
         <v>14</v>
@@ -12447,22 +12426,22 @@
     </row>
     <row r="430" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A430" s="1" t="n">
-        <v>429</v>
+        <v>432</v>
       </c>
       <c r="C430" s="1" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D430" s="1" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="E430" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I430" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="J430" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="K430" s="2" t="s">
         <v>14</v>
@@ -12470,22 +12449,22 @@
     </row>
     <row r="431" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A431" s="1" t="n">
-        <v>430</v>
+        <v>433</v>
       </c>
       <c r="C431" s="1" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D431" s="1" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="E431" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I431" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="J431" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="K431" s="2" t="s">
         <v>14</v>
@@ -12493,22 +12472,22 @@
     </row>
     <row r="432" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A432" s="1" t="n">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="C432" s="1" t="n">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D432" s="1" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="E432" s="1" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I432" s="1" t="s">
-        <v>515</v>
+        <v>535</v>
       </c>
       <c r="J432" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="K432" s="2" t="s">
         <v>14</v>
@@ -12516,22 +12495,22 @@
     </row>
     <row r="433" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A433" s="1" t="n">
-        <v>432</v>
+        <v>435</v>
       </c>
       <c r="C433" s="1" t="n">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D433" s="1" t="s">
-        <v>533</v>
+        <v>536</v>
       </c>
       <c r="E433" s="1" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I433" s="1" t="s">
-        <v>515</v>
+        <v>535</v>
       </c>
       <c r="J433" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="K433" s="2" t="s">
         <v>14</v>
@@ -12539,22 +12518,22 @@
     </row>
     <row r="434" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A434" s="1" t="n">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="C434" s="1" t="n">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D434" s="1" t="s">
-        <v>534</v>
+        <v>537</v>
       </c>
       <c r="E434" s="1" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I434" s="1" t="s">
-        <v>515</v>
+        <v>535</v>
       </c>
       <c r="J434" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="K434" s="2" t="s">
         <v>14</v>
@@ -12562,22 +12541,22 @@
     </row>
     <row r="435" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A435" s="1" t="n">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="C435" s="1" t="n">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D435" s="1" t="s">
-        <v>535</v>
+        <v>538</v>
       </c>
       <c r="E435" s="1" t="n">
         <v>3</v>
       </c>
       <c r="I435" s="1" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="J435" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="K435" s="2" t="s">
         <v>14</v>
@@ -12585,22 +12564,22 @@
     </row>
     <row r="436" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A436" s="1" t="n">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="C436" s="1" t="n">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D436" s="1" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="E436" s="1" t="n">
         <v>3</v>
       </c>
       <c r="I436" s="1" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="J436" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="K436" s="2" t="s">
         <v>14</v>
@@ -12608,22 +12587,22 @@
     </row>
     <row r="437" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A437" s="1" t="n">
-        <v>436</v>
+        <v>439</v>
       </c>
       <c r="C437" s="1" t="n">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D437" s="1" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="E437" s="1" t="n">
         <v>3</v>
       </c>
       <c r="I437" s="1" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="J437" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="K437" s="2" t="s">
         <v>14</v>
@@ -12631,22 +12610,25 @@
     </row>
     <row r="438" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A438" s="1" t="n">
-        <v>437</v>
+        <v>440</v>
       </c>
       <c r="C438" s="1" t="n">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D438" s="1" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="E438" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="F438" s="1" t="n">
+        <v>4.5</v>
       </c>
       <c r="I438" s="1" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="J438" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="K438" s="2" t="s">
         <v>14</v>
@@ -12654,22 +12636,22 @@
     </row>
     <row r="439" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A439" s="1" t="n">
-        <v>438</v>
+        <v>441</v>
       </c>
       <c r="C439" s="1" t="n">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D439" s="1" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="E439" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I439" s="1" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="J439" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="K439" s="2" t="s">
         <v>14</v>
@@ -12677,22 +12659,22 @@
     </row>
     <row r="440" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A440" s="1" t="n">
-        <v>439</v>
+        <v>442</v>
       </c>
       <c r="C440" s="1" t="n">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D440" s="1" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="E440" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I440" s="1" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="J440" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="K440" s="2" t="s">
         <v>14</v>
@@ -12700,25 +12682,22 @@
     </row>
     <row r="441" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A441" s="1" t="n">
-        <v>440</v>
+        <v>443</v>
       </c>
       <c r="C441" s="1" t="n">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D441" s="1" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="E441" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="F441" s="1" t="n">
-        <v>4.5</v>
-      </c>
       <c r="I441" s="1" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="J441" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="K441" s="2" t="s">
         <v>14</v>
@@ -12726,22 +12705,22 @@
     </row>
     <row r="442" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A442" s="1" t="n">
-        <v>441</v>
+        <v>444</v>
       </c>
       <c r="C442" s="1" t="n">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D442" s="1" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
       <c r="E442" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I442" s="1" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="J442" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="K442" s="2" t="s">
         <v>14</v>
@@ -12749,22 +12728,25 @@
     </row>
     <row r="443" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A443" s="1" t="n">
-        <v>442</v>
+        <v>445</v>
       </c>
       <c r="C443" s="1" t="n">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D443" s="1" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="E443" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="F443" s="1" t="n">
+        <v>5.5</v>
       </c>
       <c r="I443" s="1" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="J443" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="K443" s="2" t="s">
         <v>14</v>
@@ -12772,22 +12754,22 @@
     </row>
     <row r="444" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A444" s="1" t="n">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="C444" s="1" t="n">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D444" s="1" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
       <c r="E444" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I444" s="1" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="J444" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="K444" s="2" t="s">
         <v>14</v>
@@ -12795,22 +12777,22 @@
     </row>
     <row r="445" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A445" s="1" t="n">
-        <v>444</v>
+        <v>447</v>
       </c>
       <c r="C445" s="1" t="n">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D445" s="1" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="E445" s="1" t="n">
         <v>5</v>
       </c>
       <c r="I445" s="1" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="J445" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="K445" s="2" t="s">
         <v>14</v>
@@ -12818,25 +12800,22 @@
     </row>
     <row r="446" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A446" s="1" t="n">
-        <v>445</v>
+        <v>448</v>
       </c>
       <c r="C446" s="1" t="n">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D446" s="1" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="E446" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="F446" s="1" t="n">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="I446" s="1" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="J446" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="K446" s="2" t="s">
         <v>14</v>
@@ -12844,22 +12823,22 @@
     </row>
     <row r="447" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A447" s="1" t="n">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="C447" s="1" t="n">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D447" s="1" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="E447" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I447" s="1" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="J447" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="K447" s="2" t="s">
         <v>14</v>
@@ -12867,96 +12846,30 @@
     </row>
     <row r="448" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A448" s="1" t="n">
-        <v>447</v>
+        <v>450</v>
       </c>
       <c r="C448" s="1" t="n">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D448" s="1" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="E448" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I448" s="1" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="J448" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="K448" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="449" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A449" s="1" t="n">
-        <v>448</v>
-      </c>
-      <c r="C449" s="1" t="n">
-        <v>49</v>
-      </c>
-      <c r="D449" s="1" t="s">
-        <v>550</v>
-      </c>
-      <c r="E449" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="I449" s="1" t="s">
-        <v>536</v>
-      </c>
-      <c r="J449" s="1" t="s">
-        <v>499</v>
-      </c>
-      <c r="K449" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="450" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A450" s="1" t="n">
-        <v>449</v>
-      </c>
-      <c r="C450" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="D450" s="1" t="s">
-        <v>551</v>
-      </c>
-      <c r="E450" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="I450" s="1" t="s">
-        <v>536</v>
-      </c>
-      <c r="J450" s="1" t="s">
-        <v>499</v>
-      </c>
-      <c r="K450" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="451" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A451" s="1" t="n">
-        <v>450</v>
-      </c>
-      <c r="C451" s="1" t="n">
-        <v>51</v>
-      </c>
-      <c r="D451" s="1" t="s">
-        <v>552</v>
-      </c>
-      <c r="E451" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="I451" s="1" t="s">
-        <v>536</v>
-      </c>
-      <c r="J451" s="1" t="s">
-        <v>499</v>
-      </c>
-      <c r="K451" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>